<commit_message>
1115 ASG 1~2 ver 分析 ok
重複的steps會被記錄到ASG.step_list上，以前重複的只記錄最後一個step (src, dst, edgename) (v1 v2皆8007步)
</commit_message>
<xml_diff>
--- a/C ASG/1108 Dofloo單樣本統計/1115_node_statistics.xlsx
+++ b/C ASG/1108 Dofloo單樣本統計/1115_node_statistics.xlsx
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -498,7 +498,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -516,7 +516,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -534,7 +534,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -570,7 +570,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -588,11 +588,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -624,7 +624,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -642,7 +642,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>204</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>17</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17">
@@ -750,11 +750,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23">
@@ -840,7 +840,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -858,7 +858,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -876,7 +876,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -894,7 +894,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -912,7 +912,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -930,7 +930,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30">
@@ -966,7 +966,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>407</v>
+        <v>573</v>
       </c>
     </row>
     <row r="40">
@@ -1164,11 +1164,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66">
@@ -1636,7 +1636,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74">
@@ -1776,11 +1776,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2028,7 +2028,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2284,7 +2284,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104">
@@ -2514,11 +2514,11 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -2550,7 +2550,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -2658,11 +2658,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -2712,7 +2712,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -2784,7 +2784,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -2874,7 +2874,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -2946,7 +2946,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -2964,7 +2964,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144">
@@ -3018,11 +3018,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D145" t="n">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -3162,11 +3162,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -3306,7 +3306,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D161" t="n">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D168" t="n">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D169" t="n">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D170" t="n">
@@ -3508,7 +3508,7 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172">
@@ -3522,11 +3522,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -3612,7 +3612,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -3684,11 +3684,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -3774,7 +3774,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -3882,7 +3882,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -3900,7 +3900,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D193" t="n">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D194" t="n">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D195" t="n">
@@ -3954,7 +3954,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -3972,7 +3972,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -3990,7 +3990,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -4260,11 +4260,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -4296,7 +4296,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -4386,7 +4386,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -4404,11 +4404,11 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222">
@@ -4422,7 +4422,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D222" t="n">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D223" t="n">
@@ -4458,7 +4458,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -4512,7 +4512,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -4656,7 +4656,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -4674,7 +4674,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -4786,7 +4786,7 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>16</v>
+        <v>6822</v>
       </c>
     </row>
     <row r="243">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D245" t="n">
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>1</v>
+        <v>186</v>
       </c>
     </row>
     <row r="248">
@@ -4894,7 +4894,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="D249" t="n">
-        <v>6</v>
+        <v>418</v>
       </c>
     </row>
     <row r="250">
@@ -4930,7 +4930,7 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>2</v>
+        <v>336</v>
       </c>
     </row>
     <row r="251">
@@ -4944,7 +4944,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>2</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="253">
@@ -4984,7 +4984,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
     </row>
     <row r="254">
@@ -5002,7 +5002,7 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>1</v>
+        <v>300</v>
       </c>
     </row>
     <row r="255">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -5034,7 +5034,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D256" t="n">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -5074,7 +5074,7 @@
         </is>
       </c>
       <c r="D258" t="n">
-        <v>2</v>
+        <v>894</v>
       </c>
     </row>
     <row r="259">
@@ -5088,11 +5088,11 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260">
@@ -5106,11 +5106,11 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>1</v>
+        <v>296</v>
       </c>
     </row>
     <row r="261">
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="262">
@@ -5142,7 +5142,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D262" t="n">
@@ -5160,7 +5160,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -5218,7 +5218,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -5236,7 +5236,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -5250,11 +5250,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>mem</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>78</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5">
@@ -5326,7 +5326,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>180</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9">
@@ -5344,7 +5344,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10">
@@ -5380,7 +5380,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -5416,7 +5416,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
@@ -5434,7 +5434,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
@@ -5452,7 +5452,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
@@ -5614,7 +5614,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>335</v>
+        <v>573</v>
       </c>
     </row>
     <row r="25">
@@ -5650,7 +5650,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27">
@@ -5668,7 +5668,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28">
@@ -5686,7 +5686,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29">
@@ -5704,7 +5704,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
@@ -5758,7 +5758,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33">
@@ -5794,7 +5794,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
@@ -5830,7 +5830,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -5848,7 +5848,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
@@ -5884,7 +5884,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
@@ -6172,7 +6172,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56">
@@ -6190,7 +6190,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
@@ -6478,7 +6478,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>13</v>
+        <v>6822</v>
       </c>
     </row>
     <row r="73">
@@ -6532,7 +6532,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76">
@@ -6550,7 +6550,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77">
@@ -6568,7 +6568,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>6</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78">
@@ -6586,7 +6586,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79">
@@ -6604,7 +6604,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>2</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="80">
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81">
@@ -6640,7 +6640,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82">
@@ -6658,7 +6658,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>2</v>
+        <v>894</v>
       </c>
     </row>
     <row r="83">
@@ -6676,7 +6676,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>